<commit_message>
Final small fixes ... before I break something ...
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pecata\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pecata\Documents\Programming\TeamWorks\Angular-Teamwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>https://github.com/Petko-Petkov/AngularTeamwork</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -685,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -773,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -793,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -853,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -865,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -877,7 +880,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -973,7 +976,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
@@ -1064,7 +1067,9 @@
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1074,7 +1079,9 @@
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" s="7" t="s">
         <v>28</v>
       </c>
@@ -1084,7 +1091,9 @@
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1094,7 +1103,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1104,7 +1115,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1114,7 +1127,9 @@
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
@@ -1124,7 +1139,9 @@
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1134,7 +1151,9 @@
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1163,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1175,9 @@
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1164,7 +1187,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
@@ -1174,7 +1199,9 @@
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
@@ -1184,7 +1211,9 @@
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
@@ -1194,7 +1223,9 @@
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
@@ -1204,7 +1235,9 @@
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
@@ -1214,7 +1247,9 @@
       <c r="B49" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
@@ -1224,7 +1259,9 @@
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>
@@ -1236,7 +1273,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>